<commit_message>
Cleans up names for the main input file
</commit_message>
<xml_diff>
--- a/docs/DataDictionary.xlsx
+++ b/docs/DataDictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1620" windowWidth="20960" windowHeight="14300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data Classified" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="300">
   <si>
     <t>Data ID</t>
   </si>
@@ -906,6 +906,36 @@
   </si>
   <si>
     <t>KEEP</t>
+  </si>
+  <si>
+    <t>category_few_letters</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>loc</t>
+  </si>
+  <si>
+    <t>nbrhud</t>
+  </si>
+  <si>
+    <t>wea</t>
+  </si>
+  <si>
+    <t>mos</t>
+  </si>
+  <si>
+    <t>ses</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>part</t>
+  </si>
+  <si>
+    <t>Cleaned var names - intermediate step</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1330,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1328,46 +1358,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2267,8 +2257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3062,1175 +3052,1639 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B69" sqref="B69"/>
+      <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="17"/>
-    <col min="7" max="16384" width="8.83203125" style="13"/>
+    <col min="1" max="1" width="20.33203125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="28.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="13" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="17"/>
+    <col min="9" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="13" t="s">
-        <v>79</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="13" t="str">
+        <f>_xlfn.CONCAT(E2,"_",B2,"=",B2)</f>
+        <v>t_date=date</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>79</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="str">
+        <f t="shared" ref="A3:A66" si="0">_xlfn.CONCAT(E3,"_",B3,"=",B3)</f>
+        <v>t_yr=yr</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>t_mo=mo</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>t_day=day</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="D5" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="G5" s="17" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>t_qtr=qtr</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="D6" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="G6" s="17" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>t_wk=wk</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="E7" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="G7" s="17" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>t_day.of.yr=day.of.yr</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="C8" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="D8" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="E8" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="G8" s="17" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>t_day.of.wk=day.of.wk</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="C9" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="D9" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="E9" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>t_day.of.wk.name=day.of.wk.name</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="C10" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="E10" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="G10" s="17" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>t_eval.day=eval.day</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="D11" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="E11" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="G11" s="17" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>t_eval.wk=eval.wk</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="C12" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="D12" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="E12" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="G12" s="17" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>part_train=train</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="C13" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="E13" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="G13" s="17" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>part_validate=validate</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="C14" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="D14" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="E14" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="G14" s="17" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>part_test=test</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="C15" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="D15" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="E15" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="G15" s="17" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>part_partition=partition</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="C16" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="D16" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="E16" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="F16" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="G16" s="17" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>trap_trap.name=trap.name</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="C17" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="D17" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="E17" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="F17" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" s="17" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>loc_lat=lat</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="C18" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="D18" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="E18" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="F18" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="G18" s="17" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="13" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>loc_lng=lng</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="C19" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="D19" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="E19" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="F19" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="G19" s="17" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="13" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>loc_lat.lng.src=lat.lng.src</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="C20" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="D20" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="E20" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="G20" s="17" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>trap_satellite.ind=satellite.ind</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="C21" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="D21" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="E21" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="F21" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" s="17" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="13" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A22" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>loc_ZCTA5CE10=ZCTA5CE10</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="C22" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="D22" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="E22" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="F22" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="G22" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="13" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>loc_BlkGrp.geoid=BlkGrp.geoid</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="C23" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="D23" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="E23" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="F23" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="G23" s="17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="13" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>loc_Tract.geoid=Tract.geoid</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="C24" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="D24" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="E24" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="F24" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="G24" s="17" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="13" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>loc_community=community</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="C25" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="D25" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="E25" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="F25" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="G25" s="17" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="13" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>zone_zone_class=zone_class</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="C26" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="D26" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="E26" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="F26" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="G26" s="17" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>zone_zone_type=zone_type</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="C27" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="D27" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="E27" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="F27" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="G27" s="17" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A28" s="13" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>ses_LT_HS_pct__BlkGrp2017=LT_HS_pct__BlkGrp2017</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="C28" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="D28" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="E28" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="F28" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="G28" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="H28" s="17" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29" s="13" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>ses_median_HHInc__BlkGrp2017=median_HHInc__BlkGrp2017</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="C29" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="D29" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="E29" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="F29" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="G29" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="H29" s="17" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30" s="13" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>ses_LT_Pov_pct__BlkGrp2017=LT_Pov_pct__BlkGrp2017</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="C30" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="D30" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="E30" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="F30" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="G30" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="H30" s="17" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>ses_LT_HS_pct__Tract2017=LT_HS_pct__Tract2017</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="C31" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="D31" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="E31" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="F31" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="G31" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="H31" s="17" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A32" s="13" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>ses_median_HHInc__Tract2017=median_HHInc__Tract2017</v>
+      </c>
+      <c r="B32" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="C32" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="D32" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="E32" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="F32" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="G32" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="H32" s="17" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="13" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A33" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>ses_LT_Pov_pct__Tract2017=LT_Pov_pct__Tract2017</v>
+      </c>
+      <c r="B33" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="C33" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="D33" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="E33" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="F33" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="G33" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="F33" s="17" t="s">
+      <c r="H33" s="17" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34" s="13" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A34" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>trap_trap_type=trap_type</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="C34" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="D34" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="E34" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="F34" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34" s="17" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="13" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A35" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_erraticus.NumMosquitos=erraticus.NumMosquitos</v>
+      </c>
+      <c r="B35" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="C35" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="D35" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="E35" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F35" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="G35" s="17" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="13" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A36" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_pipiens.NumMosquitos=pipiens.NumMosquitos</v>
+      </c>
+      <c r="B36" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="C36" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="D36" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="E36" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F36" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="G36" s="17" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="13" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A37" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_pipiens_restuans.NumMosquitos=pipiens_restuans.NumMosquitos</v>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="C37" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="D37" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="E37" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F37" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="G37" s="17" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="13" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A38" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_restuans.NumMosquitos=restuans.NumMosquitos</v>
+      </c>
+      <c r="B38" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="C38" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="D38" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="E38" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F38" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="G38" s="17" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39" s="13" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A39" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_salinarius.NumMosquitos=salinarius.NumMosquitos</v>
+      </c>
+      <c r="B39" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="C39" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="D39" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="E39" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F39" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="G39" s="17" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A40" s="13" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A40" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_tarsalis.NumMosquitos=tarsalis.NumMosquitos</v>
+      </c>
+      <c r="B40" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="C40" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="D40" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="E40" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F40" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="G40" s="17" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A41" s="13" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A41" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_territans.NumMosquitos=territans.NumMosquitos</v>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="C41" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="D41" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="E41" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F41" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="G41" s="17" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42" s="13" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A42" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_unspecified.NumMosquitos=unspecified.NumMosquitos</v>
+      </c>
+      <c r="B42" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="C42" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="D42" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="E42" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F42" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="G42" s="17" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="15" t="s">
+    <row r="43" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_tot.NumMosquitos=tot.NumMosquitos</v>
+      </c>
+      <c r="B43" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="C43" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="D43" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="E43" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F43" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="G43" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="F43" s="18"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44" s="13" t="s">
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A44" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_erraticus.WnvPresent=erraticus.WnvPresent</v>
+      </c>
+      <c r="B44" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="C44" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="D44" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="E44" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F44" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="G44" s="17" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45" s="13" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A45" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_pipiens.WnvPresent=pipiens.WnvPresent</v>
+      </c>
+      <c r="B45" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="C45" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="D45" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="E45" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F45" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="G45" s="17" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="13" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A46" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_pipiens_restuans.WnvPresent=pipiens_restuans.WnvPresent</v>
+      </c>
+      <c r="B46" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="C46" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="D46" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="E46" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F46" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E46" s="17" t="s">
+      <c r="G46" s="17" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A47" s="13" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A47" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_restuans.WnvPresent=restuans.WnvPresent</v>
+      </c>
+      <c r="B47" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="C47" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="D47" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="E47" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F47" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E47" s="17" t="s">
+      <c r="G47" s="17" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A48" s="13" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A48" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_salinarius.WnvPresent=salinarius.WnvPresent</v>
+      </c>
+      <c r="B48" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="C48" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="D48" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="E48" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F48" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="G48" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="13" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A49" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_tarsalis.WnvPresent=tarsalis.WnvPresent</v>
+      </c>
+      <c r="B49" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="C49" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="D49" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="E49" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F49" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="G49" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="13" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A50" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_territans.WnvPresent=territans.WnvPresent</v>
+      </c>
+      <c r="B50" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="C50" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="D50" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="E50" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F50" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E50" s="17" t="s">
+      <c r="G50" s="17" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="13" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A51" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_unspecified.WnvPresent=unspecified.WnvPresent</v>
+      </c>
+      <c r="B51" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="C51" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="D51" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="E51" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F51" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E51" s="17" t="s">
+      <c r="G51" s="17" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="15" t="s">
+    <row r="52" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>mos_any.WnvPresent=any.WnvPresent</v>
+      </c>
+      <c r="B52" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="C52" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="D52" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="E52" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="F52" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="E52" s="18" t="s">
+      <c r="G52" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="F52" s="18"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="13" t="s">
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A53" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>nbrhud_comm.180d.violation.cnt=comm.180d.violation.cnt</v>
+      </c>
+      <c r="B53" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="C53" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="D53" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="E53" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="F53" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="G53" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="13" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A54" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>nbrhud_BlkGrp.180d.violation.cnt=BlkGrp.180d.violation.cnt</v>
+      </c>
+      <c r="B54" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="C54" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="D54" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="E54" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="F54" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="G54" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="13" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A55" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>nbrhud_zcta.180d.violation.cnt=zcta.180d.violation.cnt</v>
+      </c>
+      <c r="B55" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="C55" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="D55" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="E55" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="F55" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="E55" s="17" t="s">
+      <c r="G55" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A56" s="13" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A56" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>nbrhud_comm.180d.vacancies.cnt=comm.180d.vacancies.cnt</v>
+      </c>
+      <c r="B56" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="C56" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="D56" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="D56" s="13" t="s">
+      <c r="E56" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="F56" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="G56" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A57" s="13" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A57" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>nbrhud_BlkGrp.180d.vacancies.cnt=BlkGrp.180d.vacancies.cnt</v>
+      </c>
+      <c r="B57" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="C57" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="D57" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="E57" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="F57" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="E57" s="17" t="s">
+      <c r="G57" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="13" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A58" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>nbrhud_zcta.180d.vacancies.cnt=zcta.180d.vacancies.cnt</v>
+      </c>
+      <c r="B58" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="C58" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="D58" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="E58" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="F58" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="E58" s="17" t="s">
+      <c r="G58" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A59" s="13" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A59" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>wea_USW00014819_PRCP=USW00014819_PRCP</v>
+      </c>
+      <c r="B59" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="C59" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="D59" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="E59" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="F59" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="G59" s="17" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A60" s="13" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A60" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>wea_USW00014819_tavg2=USW00014819_tavg2</v>
+      </c>
+      <c r="B60" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="C60" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="D60" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D60" s="13" t="s">
+      <c r="E60" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="F60" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="G60" s="17" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A61" s="13" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A61" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>wea_USW00014819_TMAX=USW00014819_TMAX</v>
+      </c>
+      <c r="B61" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="C61" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="D61" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="E61" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="F61" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E61" s="17" t="s">
+      <c r="G61" s="17" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A62" s="13" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A62" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>wea_USW00014819_TMIN=USW00014819_TMIN</v>
+      </c>
+      <c r="B62" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="C62" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="D62" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="E62" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="F62" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="G62" s="17" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A63" s="13" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A63" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>wea_USW00094846_PRCP=USW00094846_PRCP</v>
+      </c>
+      <c r="B63" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="C63" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="D63" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="E63" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="F63" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E63" s="17" t="s">
+      <c r="G63" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="F63" s="17" t="s">
+      <c r="H63" s="17" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A64" s="13" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A64" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>wea_USW00094846_tavg2=USW00094846_tavg2</v>
+      </c>
+      <c r="B64" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="C64" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="D64" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D64" s="13" t="s">
+      <c r="E64" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="F64" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E64" s="17" t="s">
+      <c r="G64" s="17" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="13" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A65" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>wea_USW00094846_TMAX=USW00094846_TMAX</v>
+      </c>
+      <c r="B65" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="C65" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="D65" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="E65" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="F65" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E65" s="17" t="s">
+      <c r="G65" s="17" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" s="13" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A66" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>wea_USW00094846_TMIN=USW00094846_TMIN</v>
+      </c>
+      <c r="B66" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="C66" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="D66" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D66" s="13" t="s">
+      <c r="E66" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="F66" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E66" s="17" t="s">
+      <c r="G66" s="17" t="s">
         <v>225</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>